<commit_message>
Analog Pins, ADC, Speaker Frequency with Potmeter Lab
</commit_message>
<xml_diff>
--- a/Documentation/tasks.xlsx
+++ b/Documentation/tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E58E5D80-55E0-4F54-9583-7470351FA436}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -60,13 +60,55 @@
   </si>
   <si>
     <t>The fundamental idea and some conceptualisation and research on existing inventions</t>
+  </si>
+  <si>
+    <t>Arduino Tutorial</t>
+  </si>
+  <si>
+    <t>Arduino Electronic Basics - Voltagies and Currents</t>
+  </si>
+  <si>
+    <t>Arduino Electronic Basics - Resistance and Microchip</t>
+  </si>
+  <si>
+    <t>Arduino Electronic Basics - First Circuits and Lab</t>
+  </si>
+  <si>
+    <t>Arduino Electronic Basics - Analog and Digital Signal and Components</t>
+  </si>
+  <si>
+    <t>Arduino Programmin Basics - Serial, PinMode, Basic C++ and Lab: LED Series</t>
+  </si>
+  <si>
+    <t>Arduino Programmin Basics - Functions and LED State Lab</t>
+  </si>
+  <si>
+    <t>27.09.2022</t>
+  </si>
+  <si>
+    <t>29.09.2022</t>
+  </si>
+  <si>
+    <t>30.09.2022</t>
+  </si>
+  <si>
+    <t>28.09.2022</t>
+  </si>
+  <si>
+    <t>01.10.2022</t>
+  </si>
+  <si>
+    <t>Arduino Programmin Basics - 4 Different LED and Speaker Lab Project</t>
+  </si>
+  <si>
+    <t>Arduino Programmin Basics - Analog PINS, ADC, Speaker Frequency with Potmeter Lab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +120,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,6 +162,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,19 +477,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="91.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="155.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -477,7 +526,150 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>130</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="4">
+        <f>SUM(D2:D7) / 60</f>
+        <v>8.9166666666666661</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>